<commit_message>
chore: clear data from example xlsx files
</commit_message>
<xml_diff>
--- a/public/xlsx/create-input-from-file.xlsx
+++ b/public/xlsx/create-input-from-file.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Develop\Work\bstock\public\xlsx\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD060803-F091-4F84-81FB-154339812E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Planilha1"/>
+    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Nome</t>
   </si>
@@ -24,16 +30,15 @@
   <si>
     <t>Unidade de Medida</t>
   </si>
-  <si>
-    <t>kg</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -47,6 +52,14 @@
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -76,26 +89,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -106,10 +119,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -147,71 +160,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -239,7 +252,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -262,11 +275,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -275,13 +288,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -291,7 +304,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -300,7 +313,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -309,7 +322,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -317,10 +330,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -385,22 +398,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="3" width="14.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="14.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="17.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -411,16 +426,19 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
+    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="4"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" s="3"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Erro de Validação!" error="O dado inserido não corresponde a um valor decimal." prompt="Use a virgula para valores decimais." sqref="B2:B1048576" xr:uid="{EAFBA612-192D-4A66-BF8C-9010B9D6DD8A}">
+      <formula1>0</formula1>
+      <formula2>10000000</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: show more details about product and input on their pages
</commit_message>
<xml_diff>
--- a/public/xlsx/create-input-from-file.xlsx
+++ b/public/xlsx/create-input-from-file.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Develop\Work\bstock\public\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD060803-F091-4F84-81FB-154339812E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C5B30E-7AC8-419C-BE0D-E0A1D684BF8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
   <si>
     <t>Nome</t>
   </si>
@@ -29,6 +29,69 @@
   </si>
   <si>
     <t>Unidade de Medida</t>
+  </si>
+  <si>
+    <t>Microcontrolador (ESP32)</t>
+  </si>
+  <si>
+    <t>un</t>
+  </si>
+  <si>
+    <t>Módulo GPS (u-blox NEO-6M)</t>
+  </si>
+  <si>
+    <t>Módulo GSM (SIM800L)</t>
+  </si>
+  <si>
+    <t>Antena GPS</t>
+  </si>
+  <si>
+    <t>Antena GSM</t>
+  </si>
+  <si>
+    <t>Bateria Li-ion (2000mAh)</t>
+  </si>
+  <si>
+    <t>Carregador de bateria (TP4056)</t>
+  </si>
+  <si>
+    <t>Capacitores (10uF)</t>
+  </si>
+  <si>
+    <t>Resistores (10kΩ)</t>
+  </si>
+  <si>
+    <t>Sensor de temperatura (DHT11)</t>
+  </si>
+  <si>
+    <t>Sensor de movimento (MPU6050)</t>
+  </si>
+  <si>
+    <t>Conector Micro USB</t>
+  </si>
+  <si>
+    <t>PCB (Placa de Circuito Impresso)</t>
+  </si>
+  <si>
+    <t>Encapsulamento plástico</t>
+  </si>
+  <si>
+    <t>Botão de Reset</t>
+  </si>
+  <si>
+    <t>LEDs indicadores</t>
+  </si>
+  <si>
+    <t>Diodos (1N4007)</t>
+  </si>
+  <si>
+    <t>Cristal Oscilador (16MHz)</t>
+  </si>
+  <si>
+    <t>Fios de conexão</t>
+  </si>
+  <si>
+    <t>Transformador DC-DC (LM2596)</t>
   </si>
 </sst>
 </file>
@@ -38,7 +101,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -52,14 +115,6 @@
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -89,14 +144,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,17 +469,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -427,18 +495,236 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="4"/>
+      <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3">
+        <v>50</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B3" s="3"/>
+      <c r="A3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="4">
+        <v>40</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3">
+        <v>35</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="3">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="3">
+        <v>30</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="3">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="3">
+        <v>15</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="3">
+        <v>20</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="3">
+        <v>2</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="3">
+        <v>15</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="3">
+        <v>25</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="3">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="3">
+        <v>10</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations xWindow="227" yWindow="362" count="2">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Erro de Validação!" error="O dado inserido não corresponde a um valor decimal." prompt="Use a virgula para valores decimais." sqref="B2:B1048576" xr:uid="{EAFBA612-192D-4A66-BF8C-9010B9D6DD8A}">
       <formula1>0</formula1>
       <formula2>10000000</formula2>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{54278D39-0FBC-4B6D-9640-53908DF8D241}">
+      <formula1>"cm, m, kg, g, ml, l, un"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add more props on input definition
</commit_message>
<xml_diff>
--- a/public/xlsx/create-input-from-file.xlsx
+++ b/public/xlsx/create-input-from-file.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Develop\Work\bstock\public\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C5B30E-7AC8-419C-BE0D-E0A1D684BF8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61DA348A-902D-41D5-B34A-DE88081E4245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="160">
   <si>
     <t>Nome</t>
   </si>
@@ -92,6 +92,414 @@
   </si>
   <si>
     <t>Transformador DC-DC (LM2596)</t>
+  </si>
+  <si>
+    <t>Categoria</t>
+  </si>
+  <si>
+    <t>Part Number 1</t>
+  </si>
+  <si>
+    <t>Part Number 2</t>
+  </si>
+  <si>
+    <t>Part Number 3</t>
+  </si>
+  <si>
+    <t>Nome Fornecedor 1</t>
+  </si>
+  <si>
+    <t>Nome Fornecedor 2</t>
+  </si>
+  <si>
+    <t>Nome Fornecedor 3</t>
+  </si>
+  <si>
+    <t>ids</t>
+  </si>
+  <si>
+    <t>mdm</t>
+  </si>
+  <si>
+    <t>cis</t>
+  </si>
+  <si>
+    <t>com</t>
+  </si>
+  <si>
+    <t>cht</t>
+  </si>
+  <si>
+    <t>bat</t>
+  </si>
+  <si>
+    <t>cas</t>
+  </si>
+  <si>
+    <t>dis</t>
+  </si>
+  <si>
+    <t>ant</t>
+  </si>
+  <si>
+    <t>pcb</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
+    <t>004</t>
+  </si>
+  <si>
+    <t>005</t>
+  </si>
+  <si>
+    <t>006</t>
+  </si>
+  <si>
+    <t>007</t>
+  </si>
+  <si>
+    <t>008</t>
+  </si>
+  <si>
+    <t>009</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>012</t>
+  </si>
+  <si>
+    <t>013</t>
+  </si>
+  <si>
+    <t>014</t>
+  </si>
+  <si>
+    <t>015</t>
+  </si>
+  <si>
+    <t>016</t>
+  </si>
+  <si>
+    <t>017</t>
+  </si>
+  <si>
+    <t>018</t>
+  </si>
+  <si>
+    <t>019</t>
+  </si>
+  <si>
+    <t>020</t>
+  </si>
+  <si>
+    <t>Fornecedor 1</t>
+  </si>
+  <si>
+    <t>Fornecedor 2</t>
+  </si>
+  <si>
+    <t>Fornecedor 3</t>
+  </si>
+  <si>
+    <t>Fornecedor 4</t>
+  </si>
+  <si>
+    <t>Fornecedor 5</t>
+  </si>
+  <si>
+    <t>Fornecedor 6</t>
+  </si>
+  <si>
+    <t>Fornecedor 7</t>
+  </si>
+  <si>
+    <t>Fornecedor 8</t>
+  </si>
+  <si>
+    <t>Fornecedor 9</t>
+  </si>
+  <si>
+    <t>Fornecedor 10</t>
+  </si>
+  <si>
+    <t>Fornecedor 11</t>
+  </si>
+  <si>
+    <t>Fornecedor 12</t>
+  </si>
+  <si>
+    <t>Fornecedor 13</t>
+  </si>
+  <si>
+    <t>Fornecedor 14</t>
+  </si>
+  <si>
+    <t>Fornecedor 15</t>
+  </si>
+  <si>
+    <t>Fornecedor 16</t>
+  </si>
+  <si>
+    <t>Fornecedor 17</t>
+  </si>
+  <si>
+    <t>Fornecedor 18</t>
+  </si>
+  <si>
+    <t>Fornecedor 19</t>
+  </si>
+  <si>
+    <t>Fornecedor 20</t>
+  </si>
+  <si>
+    <t>021</t>
+  </si>
+  <si>
+    <t>022</t>
+  </si>
+  <si>
+    <t>023</t>
+  </si>
+  <si>
+    <t>024</t>
+  </si>
+  <si>
+    <t>025</t>
+  </si>
+  <si>
+    <t>026</t>
+  </si>
+  <si>
+    <t>027</t>
+  </si>
+  <si>
+    <t>028</t>
+  </si>
+  <si>
+    <t>029</t>
+  </si>
+  <si>
+    <t>030</t>
+  </si>
+  <si>
+    <t>031</t>
+  </si>
+  <si>
+    <t>032</t>
+  </si>
+  <si>
+    <t>033</t>
+  </si>
+  <si>
+    <t>034</t>
+  </si>
+  <si>
+    <t>035</t>
+  </si>
+  <si>
+    <t>036</t>
+  </si>
+  <si>
+    <t>037</t>
+  </si>
+  <si>
+    <t>038</t>
+  </si>
+  <si>
+    <t>039</t>
+  </si>
+  <si>
+    <t>040</t>
+  </si>
+  <si>
+    <t>041</t>
+  </si>
+  <si>
+    <t>042</t>
+  </si>
+  <si>
+    <t>043</t>
+  </si>
+  <si>
+    <t>044</t>
+  </si>
+  <si>
+    <t>045</t>
+  </si>
+  <si>
+    <t>046</t>
+  </si>
+  <si>
+    <t>047</t>
+  </si>
+  <si>
+    <t>048</t>
+  </si>
+  <si>
+    <t>049</t>
+  </si>
+  <si>
+    <t>050</t>
+  </si>
+  <si>
+    <t>051</t>
+  </si>
+  <si>
+    <t>052</t>
+  </si>
+  <si>
+    <t>053</t>
+  </si>
+  <si>
+    <t>054</t>
+  </si>
+  <si>
+    <t>055</t>
+  </si>
+  <si>
+    <t>056</t>
+  </si>
+  <si>
+    <t>057</t>
+  </si>
+  <si>
+    <t>058</t>
+  </si>
+  <si>
+    <t>059</t>
+  </si>
+  <si>
+    <t>060</t>
+  </si>
+  <si>
+    <t>Fornecedor 21</t>
+  </si>
+  <si>
+    <t>Fornecedor 22</t>
+  </si>
+  <si>
+    <t>Fornecedor 23</t>
+  </si>
+  <si>
+    <t>Fornecedor 24</t>
+  </si>
+  <si>
+    <t>Fornecedor 25</t>
+  </si>
+  <si>
+    <t>Fornecedor 26</t>
+  </si>
+  <si>
+    <t>Fornecedor 27</t>
+  </si>
+  <si>
+    <t>Fornecedor 28</t>
+  </si>
+  <si>
+    <t>Fornecedor 29</t>
+  </si>
+  <si>
+    <t>Fornecedor 30</t>
+  </si>
+  <si>
+    <t>Fornecedor 31</t>
+  </si>
+  <si>
+    <t>Fornecedor 32</t>
+  </si>
+  <si>
+    <t>Fornecedor 33</t>
+  </si>
+  <si>
+    <t>Fornecedor 34</t>
+  </si>
+  <si>
+    <t>Fornecedor 35</t>
+  </si>
+  <si>
+    <t>Fornecedor 36</t>
+  </si>
+  <si>
+    <t>Fornecedor 37</t>
+  </si>
+  <si>
+    <t>Fornecedor 38</t>
+  </si>
+  <si>
+    <t>Fornecedor 39</t>
+  </si>
+  <si>
+    <t>Fornecedor 40</t>
+  </si>
+  <si>
+    <t>Fornecedor 50</t>
+  </si>
+  <si>
+    <t>Fornecedor 41</t>
+  </si>
+  <si>
+    <t>Fornecedor 42</t>
+  </si>
+  <si>
+    <t>Fornecedor 43</t>
+  </si>
+  <si>
+    <t>Fornecedor 44</t>
+  </si>
+  <si>
+    <t>Fornecedor 45</t>
+  </si>
+  <si>
+    <t>Fornecedor 46</t>
+  </si>
+  <si>
+    <t>Fornecedor 47</t>
+  </si>
+  <si>
+    <t>Fornecedor 48</t>
+  </si>
+  <si>
+    <t>Fornecedor 49</t>
+  </si>
+  <si>
+    <t>Fornecedor 51</t>
+  </si>
+  <si>
+    <t>Fornecedor 52</t>
+  </si>
+  <si>
+    <t>Fornecedor 53</t>
+  </si>
+  <si>
+    <t>Fornecedor 54</t>
+  </si>
+  <si>
+    <t>Fornecedor 55</t>
+  </si>
+  <si>
+    <t>Fornecedor 56</t>
+  </si>
+  <si>
+    <t>Fornecedor 57</t>
+  </si>
+  <si>
+    <t>Fornecedor 58</t>
+  </si>
+  <si>
+    <t>Fornecedor 59</t>
   </si>
 </sst>
 </file>
@@ -101,7 +509,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,6 +523,20 @@
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -155,14 +577,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -469,259 +891,711 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="28.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3">
+      <c r="C2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="I2" s="3">
         <v>50</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="J2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4">
+      <c r="C3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="I3" s="3">
         <v>40</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="J3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3">
+      <c r="C4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="I4" s="3">
         <v>35</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="J4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="3">
+      <c r="C5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="I5" s="3">
         <v>10</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="J5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="3">
+      <c r="C6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="I6" s="3">
         <v>8</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="J6" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3">
+      <c r="C7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="I7" s="3">
         <v>30</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="J7" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="3">
+      <c r="C8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="I8" s="3">
         <v>5</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+      <c r="J8" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="3">
+      <c r="C9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="I9" s="3">
         <v>0.1</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="J9" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="3">
+      <c r="C10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="I10" s="3">
         <v>0.05</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="J10" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="3">
+      <c r="C11" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="I11" s="3">
         <v>15</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+      <c r="J11" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="3">
+      <c r="C12" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="I12" s="3">
         <v>20</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
+      <c r="J12" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="3">
+      <c r="C13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="I13" s="3">
         <v>2</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+      <c r="J13" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="3">
+      <c r="C14" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="I14" s="3">
         <v>15</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
+      <c r="J14" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="3">
+      <c r="C15" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="I15" s="3">
         <v>25</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
+      <c r="J15" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="3">
+      <c r="C16" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="I16" s="3">
         <v>1</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
+      <c r="J16" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="3">
+      <c r="C17" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="I17" s="3">
         <v>0.5</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
+      <c r="J17" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="3">
+      <c r="C18" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="I18" s="3">
         <v>0.2</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
+      <c r="J18" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="3">
+      <c r="C19" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="I19" s="3">
         <v>1.5</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
+      <c r="J19" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="3">
+      <c r="C20" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="I20" s="3">
         <v>0.1</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
+      <c r="J20" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="3">
+      <c r="C21" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="I21" s="3">
         <v>10</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="J21" s="2" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations xWindow="227" yWindow="362" count="2">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Erro de Validação!" error="O dado inserido não corresponde a um valor decimal." prompt="Use a virgula para valores decimais." sqref="B2:B1048576" xr:uid="{EAFBA612-192D-4A66-BF8C-9010B9D6DD8A}">
+  <phoneticPr fontId="3" type="noConversion"/>
+  <dataValidations xWindow="227" yWindow="362" count="3">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Erro de Validação!" error="O dado inserido não corresponde a um valor decimal." prompt="Use a virgula para valores decimais." sqref="I2:I1048576" xr:uid="{EAFBA612-192D-4A66-BF8C-9010B9D6DD8A}">
       <formula1>0</formula1>
       <formula2>10000000</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{54278D39-0FBC-4B6D-9640-53908DF8D241}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576" xr:uid="{54278D39-0FBC-4B6D-9640-53908DF8D241}">
       <formula1>"cm, m, kg, g, ml, l, un"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{5A3E5D00-1282-4F90-BCF7-0AE714CB2B25}">
+      <formula1>"mdm,ids,cis,com,pcb,bat,cht,cas,ant,dis"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
chore: add new categories into list options
</commit_message>
<xml_diff>
--- a/public/xlsx/create-input-from-file.xlsx
+++ b/public/xlsx/create-input-from-file.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodrigo.ribeiro\Documents\bstock\bstock\public\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BWS\bstock\public\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982863F4-F2CD-4C8C-9577-68ABFAC24CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0485A2-BB42-433D-999E-1E4EB8C84292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -151,7 +151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -172,9 +172,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -485,7 +482,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,9 +573,6 @@
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C6" s="7"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J7" s="8"/>
-    </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
     </row>
@@ -593,7 +587,7 @@
       <formula1>"cm, m, kg, g, ml, l, un"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{23845CC8-30FE-4355-844D-6E5C7EE869EF}">
-      <formula1>"cap,dio,fet,swa,dcd,res,con,mod,ldo,led,sen,ind,mem,ic"</formula1>
+      <formula1>"cap,dio,fet,swa,dcd,res,con,mod,ldo,led,sen,ind,mem,ic,ant,fus,swi,trn"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>